<commit_message>
CCDB-290: Removed update relaton from the application.
</commit_message>
<xml_diff>
--- a/conf-core/src/main/webapp/resources/import-templates/ccdb_slots.xlsx
+++ b/conf-core/src/main/webapp/resources/import-templates/ccdb_slots.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -247,6 +252,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -295,7 +303,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -330,7 +338,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -722,7 +730,7 @@
       <formula1>"CONTAINER,SLOT"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A10:A1048576">
-      <formula1>"CREATE ENTITY,UPDATE ENTITY,DELETE ENTITY,CREATE PROPERTY,UPDATE PROPERTY,DELETE PROPERTY,CREATE RELATION,UPDATE RELATION,DELETE RELATION,INSTALL,UNINSTALL"</formula1>
+      <formula1>"CREATE ENTITY,UPDATE ENTITY,DELETE ENTITY,CREATE PROPERTY,UPDATE PROPERTY,DELETE PROPERTY,CREATE RELATION,DELETE RELATION,INSTALL,UNINSTALL"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>